<commit_message>
Making changes for EDI
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2022_FilteringLog_EDI.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2022_FilteringLog_EDI.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecewood/Documents/Virginia Tech/Sed Traps/2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecewood/Documents/GitHub/Reservoirs/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2539AEB-A20B-7D49-B2F6-784F63B48D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4DA627-6BEE-C947-9338-28FC69E42271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1820" windowWidth="27240" windowHeight="16440" xr2:uid="{935FE88D-5A76-9C4B-B068-21F1249E5482}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2168,8 +2168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7AD213A-FA22-B146-A187-262FE9F878FB}">
   <dimension ref="A1:K529"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K529"/>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="E213" sqref="E213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8921,7 +8921,7 @@
         <v>0.96599999999999997</v>
       </c>
       <c r="E211" s="4">
-        <v>1.7000000000000001E-2</v>
+        <v>0.107</v>
       </c>
       <c r="F211" s="4">
         <v>0.124</v>
@@ -8934,7 +8934,7 @@
       </c>
       <c r="I211" s="1">
         <f t="shared" si="3"/>
-        <v>0.107</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="J211">
         <v>14</v>

</xml_diff>

<commit_message>
Fixed 2022 filtering log so it wasnt reading in a bunch of empty cells. Then updated the filtering log csv to include 2023 data
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2022_FilteringLog_EDI.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2022_FilteringLog_EDI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlybauer/Desktop/Reservoirs/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE4541F-E2F8-514E-878F-D27B913E6C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7818A672-2099-8D43-903C-B137F2DD35F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="-20900" windowWidth="27240" windowHeight="16000" xr2:uid="{935FE88D-5A76-9C4B-B068-21F1249E5482}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{935FE88D-5A76-9C4B-B068-21F1249E5482}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2172,13 +2172,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7AD213A-FA22-B146-A187-262FE9F878FB}">
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:M529"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A530" sqref="A530:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -23490,12 +23490,6 @@
         <v>12</v>
       </c>
       <c r="M529" s="1"/>
-    </row>
-    <row r="1048576" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G1048576">
-        <f>SUM(G2:G1048575)</f>
-        <v>60734</v>
-      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C123">

</xml_diff>